<commit_message>
STX and STY operations
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -512,11 +512,11 @@
   </sheetPr>
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.11"/>
@@ -538,7 +538,11 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="false">COUNTIF(C3:O58, "I")</f>
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <f aca="false">B2-B1</f>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,7 +551,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">COUNTIF(C3:O58, "N")</f>
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,7 +2857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>116</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>20</v>
@@ -2873,7 +2877,7 @@
         <v>19</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>20</v>
@@ -2882,10 +2886,10 @@
         <v>20</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L52" s="0" t="s">
         <v>20</v>
@@ -2900,7 +2904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>118</v>
       </c>
@@ -2911,7 +2915,7 @@
         <v>20</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>19</v>
@@ -2920,7 +2924,7 @@
         <v>20</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H53" s="0" t="s">
         <v>20</v>
@@ -2929,10 +2933,10 @@
         <v>20</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L53" s="0" t="s">
         <v>20</v>

</xml_diff>